<commit_message>
data with wood and litter moisture
</commit_message>
<xml_diff>
--- a/data/example_database.xlsx
+++ b/data/example_database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="17535" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="17535" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>order</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>to wirte any observation worth mentioning</t>
+  </si>
+  <si>
+    <t>wood</t>
+  </si>
+  <si>
+    <t>amount of wood</t>
   </si>
 </sst>
 </file>
@@ -581,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE17"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -599,14 +605,14 @@
     <col min="19" max="19" width="6.375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6.375" customWidth="1"/>
     <col min="21" max="22" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18" customWidth="1"/>
-    <col min="24" max="24" width="18" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="18" customWidth="1"/>
+    <col min="25" max="25" width="18" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,31 +683,34 @@
         <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -747,12 +756,9 @@
       <c r="O2">
         <v>8</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>1</v>
       </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
       <c r="Z2">
         <v>0</v>
       </c>
@@ -768,8 +774,11 @@
       <c r="AD2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -815,9 +824,6 @@
       <c r="O3">
         <v>8</v>
       </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
       <c r="Y3">
         <v>0</v>
       </c>
@@ -825,19 +831,22 @@
         <v>0</v>
       </c>
       <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
         <v>1</v>
       </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
       <c r="AC3">
         <v>0</v>
       </c>
       <c r="AD3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -845,62 +854,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -922,10 +931,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1119,15 +1128,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>56</v>
@@ -1135,7 +1144,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>56</v>
@@ -1143,7 +1152,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>56</v>
@@ -1151,7 +1160,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>56</v>
@@ -1159,7 +1168,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>56</v>
@@ -1167,7 +1176,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>56</v>
@@ -1175,9 +1184,17 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>